<commit_message>
add to control session
</commit_message>
<xml_diff>
--- a/tableinfo.xlsx
+++ b/tableinfo.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22fbeb63e0c81cc2/デスクトップ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\15_07_kadai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{D1CEC2B6-AC0B-4440-BC00-02E9FAF1FDAD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{D5B567DC-D3BE-4293-95AB-B507DFC1CAD8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85478D2C-62D8-4CE4-87CB-0DA2175713D0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10973" xr2:uid="{C814C207-E7A4-4C80-B748-42375413C543}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>age</t>
     <phoneticPr fontId="1"/>
@@ -35,50 +35,18 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>user_book</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bookid</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>favorate</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>sysdate</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>sort</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>category</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>row</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>column</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>user_info</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>user_set</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rayout</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>user_follower</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -91,26 +59,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>user_like</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>like_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>comment</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>com_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>auther</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>abstract</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -171,7 +119,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>img_comment</t>
+    <t>user_good</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -204,12 +152,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -218,8 +181,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370A66B1-BCD4-4A44-AB46-E4784796C4AD}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
@@ -554,305 +520,185 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.7">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.7">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.7">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.7">
       <c r="A9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.7">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.7">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.7">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.7">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.7">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.7">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>